<commit_message>
refactor UI, generate report
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/SocialInsurance.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/SocialInsurance.xlsx
@@ -17,6 +17,7 @@
   <definedNames>
     <definedName name="RangeEmployee">Sheet1!$A$12:$Q$12</definedName>
     <definedName name="RangeFooterEachOffice">Sheet1!$A$13:$Q$13</definedName>
+    <definedName name="RangeFooterPage">Sheet1!$A$14:$Q$15</definedName>
     <definedName name="RangeOffice">Sheet1!$A$11:$Q$11</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>累計支給額チェックリスト</t>
   </si>
@@ -71,6 +72,25 @@
   </si>
   <si>
     <t>子供子育て拠出金</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>納入告知額</t>
+  </si>
+  <si>
+    <t xml:space="preserve">被保険者徴収額計
+</t>
+  </si>
+  <si>
+    <t>事業主負担</t>
+  </si>
+  <si>
+    <t>子供子育て拠出金…</t>
   </si>
 </sst>
 </file>
@@ -359,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -405,6 +425,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -455,6 +496,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -777,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="123" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:Q10"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="58" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -819,7 +866,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="2">
         <f ca="1">NOW()</f>
-        <v>42807.633532754633</v>
+        <v>42807.741354745369</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -842,25 +889,25 @@
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="29"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="36"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
@@ -939,68 +986,68 @@
       <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="1:17" s="6" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="36" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="36" t="s">
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="N8" s="38"/>
-      <c r="O8" s="36" t="s">
+      <c r="N8" s="45"/>
+      <c r="O8" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="41" t="s">
+      <c r="P8" s="45"/>
+      <c r="Q8" s="48" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:17" s="6" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="32"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="36" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="36" t="s">
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="39" t="s">
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="N9" s="39" t="s">
+      <c r="N9" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="P9" s="39" t="s">
+      <c r="P9" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="Q9" s="42"/>
+      <c r="Q9" s="49"/>
     </row>
     <row r="10" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
-      <c r="B10" s="35"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="11" t="s">
         <v>2</v>
       </c>
@@ -1031,11 +1078,11 @@
       <c r="L10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="43"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="50"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="17"/>
@@ -1094,11 +1141,40 @@
       <c r="P13" s="14"/>
       <c r="Q13" s="15"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B14"/>
+    <row r="14" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="30"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="28"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="52"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15"/>
+      <c r="K15" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
qpp018 report for show category item
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/SocialInsurance.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/SocialInsurance.xlsx
@@ -15,11 +15,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$Q$138</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$Q$136</definedName>
     <definedName name="RangeChildRaising">Sheet1!$A$15:$Q$15</definedName>
-    <definedName name="RangeChildRaisingManual">Sheet1!$A$19:$Q$19</definedName>
+    <definedName name="RangeChildRaisingManual">Sheet1!#REF!</definedName>
     <definedName name="RangeDeliveryNoticeAmount">Sheet1!$A$14:$Q$14</definedName>
-    <definedName name="RangeDeliveryNoticeAmountManual">Sheet1!$A$18:$Q$18</definedName>
+    <definedName name="RangeDeliveryNoticeAmountManual">Sheet1!#REF!</definedName>
     <definedName name="RangeEmployee">Sheet1!$A$17:$Q$17</definedName>
     <definedName name="RangeFooterEachOffice">Sheet1!$A$13:$Q$13</definedName>
     <definedName name="RangeOffice">Sheet1!$A$12:$Q$12</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>社員</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>事業主負担</t>
-  </si>
-  <si>
-    <t>子供子育て拠出金…</t>
   </si>
   <si>
     <t>&amp;=HEADER.nameCompany</t>
@@ -387,17 +384,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -425,126 +416,93 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -560,8 +518,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="37" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -883,390 +853,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="M15" activeCellId="3" sqref="C14:D14 H14:I14 M14:N14 M15:N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" style="6" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="9" customWidth="1"/>
-    <col min="3" max="16" width="11.33203125" style="15" customWidth="1"/>
-    <col min="17" max="17" width="15.5" style="15" customWidth="1"/>
+    <col min="1" max="1" width="13" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="7" customWidth="1"/>
+    <col min="3" max="14" width="11.33203125" style="11" customWidth="1"/>
+    <col min="15" max="15" width="12" style="11" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" style="11" customWidth="1"/>
+    <col min="17" max="17" width="15.5" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="Q1" s="12">
+        <f ca="1" xml:space="preserve"> NOW()</f>
+        <v>42842.64956435185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B2" s="4"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="Q2" s="12"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="Q1" s="16">
-        <f ca="1" xml:space="preserve"> NOW()</f>
-        <v>42815.580697337966</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B2" s="6"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="Q2" s="16"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="40"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="38" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="38" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="42" t="s">
+      <c r="B9" s="33"/>
+      <c r="C9" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="42" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="N9" s="44"/>
-      <c r="O9" s="42" t="s">
+      <c r="N9" s="36"/>
+      <c r="O9" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="55" t="s">
-        <v>23</v>
+      <c r="P9" s="36"/>
+      <c r="Q9" s="42" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="42" t="s">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="42" t="s">
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="56" t="s">
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="56" t="s">
+      <c r="N10" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="O10" s="56" t="s">
+      <c r="O10" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="P10" s="56" t="s">
+      <c r="P10" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="Q10" s="55"/>
+      <c r="Q10" s="42"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="12" t="s">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="57"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="55"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="42"/>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="20"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="16"/>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="25"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="21"/>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="50"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="45"/>
       <c r="D14" s="46"/>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="49" t="s">
+      <c r="F14" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="50"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="33" t="s">
+      <c r="G14" s="39"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="53" t="s">
+      <c r="K14" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="54"/>
+      <c r="L14" s="41"/>
       <c r="M14" s="45"/>
       <c r="N14" s="46"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="6"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="L15" s="47"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
+      <c r="B15" s="4"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="37"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
     </row>
     <row r="16" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
     </row>
     <row r="17" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="30"/>
-    </row>
-    <row r="18" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18"/>
-      <c r="E18" s="2"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18" s="58" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18"/>
-      <c r="J18" s="3"/>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="O18" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="15"/>
-    </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-      <c r="O19" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="P19" s="37"/>
-    </row>
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="26"/>
+    </row>
+    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="25">
     <mergeCell ref="Q9:Q11"/>

</xml_diff>